<commit_message>
added a seperate set of analysis looking at both mothers and fathers if alive in the same models. Added a new variable for whether parents live within the hour. Modified the written paper to reflect results.
</commit_message>
<xml_diff>
--- a/Table 1/OLS results.xlsx
+++ b/Table 1/OLS results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrissoria/Documents/Research/UCNets_Fathers_Social_Networks/Table 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CBE0A7-7A94-FA4F-A61C-E917AF7FE33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB8C5B1-9237-A640-9422-B387A27AF0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{6550F40D-81B3-4242-896E-5BF0E984F37C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>B</t>
   </si>
@@ -109,6 +109,57 @@
   </si>
   <si>
     <t>Education</t>
+  </si>
+  <si>
+    <t>0.443*</t>
+  </si>
+  <si>
+    <t>0.159***</t>
+  </si>
+  <si>
+    <t>-0.63**</t>
+  </si>
+  <si>
+    <t>0.94***</t>
+  </si>
+  <si>
+    <t>-0.902***</t>
+  </si>
+  <si>
+    <t>-0.488*</t>
+  </si>
+  <si>
+    <t>0.573**</t>
+  </si>
+  <si>
+    <t>1.284***</t>
+  </si>
+  <si>
+    <t>-0.454**</t>
+  </si>
+  <si>
+    <t>-0.692***</t>
+  </si>
+  <si>
+    <t>-0.394**</t>
+  </si>
+  <si>
+    <t>-0.536**</t>
+  </si>
+  <si>
+    <t>-1.647***</t>
+  </si>
+  <si>
+    <t>0.117***</t>
+  </si>
+  <si>
+    <t>0.091*</t>
+  </si>
+  <si>
+    <t>1.036***</t>
+  </si>
+  <si>
+    <t>-0.375*</t>
   </si>
 </sst>
 </file>
@@ -218,18 +269,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B007E7A-FF01-C047-B31E-239640A914ED}">
   <dimension ref="A2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="A2:J22"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,21 +608,21 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -604,604 +655,604 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="6">
         <v>4.4279999999999999</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <v>1.0349999999999999</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6">
         <v>2.0499999999999998</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>0.71299999999999997</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6">
         <v>2.3809999999999998</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="6">
         <v>0.752</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="6">
         <v>0.51200000000000001</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
         <v>0.308</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="E5" s="3">
-        <v>0.57299999999999995</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6">
         <v>0.21199999999999999</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="6">
         <v>-6.3E-2</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="6">
         <v>0.224</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="6">
         <v>-1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="6">
         <v>0.38200000000000001</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>0.27600000000000002</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>0.157</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>0.19</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="6">
         <v>0.23599999999999999</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="6">
         <v>0.20100000000000001</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="6">
         <v>0.06</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="6">
         <v>-4.7E-2</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <v>0.28399999999999997</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>0.19600000000000001</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="6">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="6">
         <v>0.20699999999999999</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="6">
         <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="6">
         <v>0.2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>0.309</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>-4.2000000000000003E-2</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <v>0.21299999999999999</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="6">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="6">
         <v>0.246</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="6">
         <v>0.22500000000000001</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="6">
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="6">
         <v>-0.376</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>0.20399999999999999</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>-7.3999999999999996E-2</v>
       </c>
-      <c r="E9" s="3">
-        <v>1.284</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="6">
         <v>0.34799999999999998</v>
       </c>
-      <c r="H9" s="3">
-        <v>-1.647</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="H9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="6">
         <v>0.14799999999999999</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="6">
         <v>-0.42</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.443</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6">
         <v>0.22</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="6">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="6">
         <v>0.151</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="6">
         <v>0.02</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="6">
         <v>0.36499999999999999</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="6">
         <v>0.16</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="6">
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.184</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2.7E-2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="6">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.17599999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="6">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.308</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>-0.36499999999999999</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="G12" s="6">
+        <v>-9.4E-2</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.224</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="C13" s="6">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D13" s="6">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="F13" s="6">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G13" s="6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="6">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="J13" s="6">
+        <v>7.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D14" s="6">
+        <v>-0.12</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="6">
         <v>0.159</v>
       </c>
-      <c r="C11" s="3">
-        <v>3.9E-2</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.184</v>
-      </c>
-      <c r="E11" s="3">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="F11" s="3">
-        <v>2.7E-2</v>
-      </c>
-      <c r="G11" s="3">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="I11" s="3">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="J11" s="3">
-        <v>0.17599999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.308</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E12" s="3">
-        <v>-0.36499999999999999</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="G14" s="6">
+        <v>-0.11899999999999999</v>
+      </c>
+      <c r="H14" s="6">
+        <v>-0.182</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="J14" s="6">
+        <v>-4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="6">
         <v>-9.4E-2</v>
       </c>
-      <c r="H12" s="3">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.224</v>
-      </c>
-      <c r="J12" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="C13" s="3">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F13" s="3">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="G13" s="3">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="H13" s="3">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="I13" s="3">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="J13" s="3">
-        <v>7.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="3">
-        <v>-0.63</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="D14" s="3">
-        <v>-0.12</v>
-      </c>
-      <c r="E14" s="3">
-        <v>-0.45400000000000001</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.159</v>
-      </c>
-      <c r="G14" s="3">
-        <v>-0.11899999999999999</v>
-      </c>
-      <c r="H14" s="3">
-        <v>-0.182</v>
-      </c>
-      <c r="I14" s="3">
+      <c r="C15" s="6">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="D15" s="6">
+        <v>-1.2999999999999999E-2</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="G15" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H15" s="6">
+        <v>-0.111</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.217</v>
+      </c>
+      <c r="J15" s="6">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D16" s="6">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.251</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G16" s="6">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="J16" s="6">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="E17" s="6">
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.19</v>
+      </c>
+      <c r="G17" s="6">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="J17" s="6">
+        <v>0.24299999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="D18" s="6">
+        <v>-0.17699999999999999</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.19</v>
+      </c>
+      <c r="G18" s="6">
+        <v>-0.188</v>
+      </c>
+      <c r="H18" s="6">
+        <v>-0.216</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="J18" s="6">
+        <v>-5.5E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="D19" s="6">
+        <v>-9.0999999999999998E-2</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.151</v>
+      </c>
+      <c r="G19" s="6">
+        <v>-0.10199999999999999</v>
+      </c>
+      <c r="H19" s="6">
+        <v>-9.2999999999999999E-2</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="J19" s="6">
+        <v>-2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6">
+        <v>-0.51600000000000001</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="D20" s="6">
+        <v>-5.5E-2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.254</v>
+      </c>
+      <c r="G20" s="6">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="H20" s="6">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="J20" s="6">
+        <v>-2E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="6">
+        <v>-0.47299999999999998</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="D21" s="6">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>-0.24099999999999999</v>
+      </c>
+      <c r="F21" s="6">
         <v>0.16800000000000001</v>
       </c>
-      <c r="J14" s="3">
-        <v>-4.4999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="3">
-        <v>-9.4E-2</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.29799999999999999</v>
-      </c>
-      <c r="D15" s="3">
+      <c r="G21" s="6">
+        <v>-5.6000000000000001E-2</v>
+      </c>
+      <c r="H21" s="6">
+        <v>-0.224</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="J21" s="6">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="6">
+        <v>-0.433</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.251</v>
+      </c>
+      <c r="D22" s="6">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="E22" s="6">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="G22" s="6">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="E15" s="3">
-        <v>1.4E-2</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="G15" s="3">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H15" s="3">
-        <v>-0.111</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0.217</v>
-      </c>
-      <c r="J15" s="3">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="D16" s="3">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.251</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="G16" s="3">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.23799999999999999</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="J16" s="3">
-        <v>5.1999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0.94</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.17</v>
-      </c>
-      <c r="E17" s="3">
-        <v>-9.6000000000000002E-2</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="G17" s="3">
-        <v>-2.4E-2</v>
-      </c>
-      <c r="H17" s="3">
-        <v>1.036</v>
-      </c>
-      <c r="I17" s="3">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0.24299999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="3">
-        <v>-0.90200000000000002</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="D18" s="3">
-        <v>-0.17699999999999999</v>
-      </c>
-      <c r="E18" s="3">
-        <v>-0.69199999999999995</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="G18" s="3">
-        <v>-0.188</v>
-      </c>
-      <c r="H18" s="3">
-        <v>-0.216</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="J18" s="3">
-        <v>-5.5E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="3">
-        <v>-0.48799999999999999</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="D19" s="3">
-        <v>-9.0999999999999998E-2</v>
-      </c>
-      <c r="E19" s="3">
-        <v>-0.39400000000000002</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.151</v>
-      </c>
-      <c r="G19" s="3">
-        <v>-0.10199999999999999</v>
-      </c>
-      <c r="H19" s="3">
-        <v>-9.2999999999999999E-2</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="J19" s="3">
-        <v>-2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="3">
-        <v>-0.51600000000000001</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="D20" s="3">
-        <v>-5.5E-2</v>
-      </c>
-      <c r="E20" s="3">
-        <v>-0.53600000000000003</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.254</v>
-      </c>
-      <c r="G20" s="3">
-        <v>-7.9000000000000001E-2</v>
-      </c>
-      <c r="H20" s="3">
-        <v>-1.0999999999999999E-2</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0.26800000000000002</v>
-      </c>
-      <c r="J20" s="3">
-        <v>-2E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="3">
-        <v>-0.47299999999999998</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="D21" s="3">
-        <v>-7.9000000000000001E-2</v>
-      </c>
-      <c r="E21" s="3">
-        <v>-0.24099999999999999</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="G21" s="3">
-        <v>-5.6000000000000001E-2</v>
-      </c>
-      <c r="H21" s="3">
-        <v>-0.224</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="J21" s="3">
-        <v>-4.9000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3">
-        <v>-0.433</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0.251</v>
-      </c>
-      <c r="D22" s="3">
-        <v>-7.1999999999999995E-2</v>
-      </c>
-      <c r="E22" s="3">
-        <v>-5.7000000000000002E-2</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="G22" s="3">
-        <v>-1.2999999999999999E-2</v>
-      </c>
-      <c r="H22" s="3">
-        <v>-0.375</v>
-      </c>
-      <c r="I22" s="3">
+      <c r="H22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="6">
         <v>0.182</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="6">
         <v>-0.08</v>
       </c>
     </row>

</xml_diff>